<commit_message>
Asset Mk1, Bureaucracy, Stock TKS
Asset Mk1, Bureaucracy, Stock TKS Support, Fix incorrect passes in Kerbalism configurations.
</commit_message>
<xml_diff>
--- a/Source/Completed/AssetMk1.xlsx
+++ b/Source/Completed/AssetMk1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\3D\KSP\kiwiTechTree\Source\Completed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EEEE7BF0-0190-498C-83C7-80CF10FE281E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFC0CF4E-4D9D-4353-83C5-5E53B63C33B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2190" yWindow="4540" windowWidth="26870" windowHeight="15160" xr2:uid="{CFEC3D39-50CD-4BC5-8A2D-E61E52BBE13D}"/>
+    <workbookView xWindow="4380" yWindow="5840" windowWidth="26870" windowHeight="15160" xr2:uid="{CFEC3D39-50CD-4BC5-8A2D-E61E52BBE13D}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts" sheetId="1" r:id="rId1"/>
@@ -3601,7 +3601,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>